<commit_message>
Cambio funciones por módulos
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Organización H" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Organización T'!$A$3:$H$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Organización T'!$A$3:$I$66</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
   <si>
     <t>Días laborables</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Manual de usuario y administrador</t>
-  </si>
-  <si>
-    <t>Funciones utilizadas</t>
   </si>
   <si>
     <t>Datos de entrada necesarios</t>
@@ -348,6 +345,12 @@
 Elección del vano adecuado según el radio
 Comprobación de los incrementos máximos de los vanos y su corrección. 
 Calculos necesarios para sortear todos los puntos singulares del trazado, tales como: pasos superiores bajos, pasos inferiores, pasos a nivel, obras de drenaje, viaductos, agujas, desvíos, tuneles, puentes,...</t>
+  </si>
+  <si>
+    <t>Modulos utilizados</t>
+  </si>
+  <si>
+    <t>Funciones</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,6 +640,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,13 +955,13 @@
       <selection activeCell="C3" sqref="C3:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -960,7 +969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
       <c r="C3" s="16" t="s">
         <v>16</v>
@@ -999,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1054,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>15</v>
       </c>
@@ -1075,7 +1084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1126,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1130,7 +1139,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>17</v>
       </c>
@@ -1214,7 +1223,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1227,7 +1236,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="13" t="s">
         <v>16</v>
@@ -1260,7 +1269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1309,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1381,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1385,7 +1394,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
@@ -1480,26 +1489,27 @@
   <sheetPr codeName="Hoja2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H67"/>
+  <dimension ref="A2:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" style="21" customWidth="1"/>
     <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="35" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="24" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="35" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
@@ -1507,25 +1517,28 @@
         <v>19</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>76</v>
-      </c>
       <c r="G3" s="16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <v>1</v>
       </c>
@@ -1533,664 +1546,700 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <v>3</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="26"/>
+      <c r="H8" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="26"/>
+      <c r="H9" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="26"/>
+      <c r="H14" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="26"/>
+      <c r="H15" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="I27" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="22"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="23" t="s">
+      <c r="D31" s="23"/>
+      <c r="E31" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="26"/>
+      <c r="H34" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I34" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="26"/>
+      <c r="H35" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I37" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I38" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" s="21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="25"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="26"/>
+      <c r="H41" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="25">
+        <v>4</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="25"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="25"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="25"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="25"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="25"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="25"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="25"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="25"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I48" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="25"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="25"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I50" s="21">
         <v>31</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="G8" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="G9" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23" t="s">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="25"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" s="21">
         <v>32</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="21">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="G14" s="21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="G15" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="21">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="21">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="22"/>
-    </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H31" s="21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H33" s="21">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="G34" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H34" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="G35" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H35" s="21">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H38" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H39" s="21">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="G41" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="24">
-        <v>4</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="H42" s="21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="H47" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="H48" s="21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H49" s="21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="H50" s="21">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="H51" s="21">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
-      <c r="B52" s="23"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D53" s="22"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D54" s="22"/>
+      <c r="G53" s="22"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D55" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E55" s="22"/>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E55" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="22"/>
+      <c r="H55" s="22"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H56" s="22"/>
+    </row>
+    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="21">
         <v>5</v>
       </c>
@@ -2198,30 +2247,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C58" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="22"/>
+      <c r="H58" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C59" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="E59" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F58" s="22"/>
-      <c r="G58" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C59" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="21">
         <v>6</v>
       </c>
@@ -2229,32 +2278,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="22"/>
       <c r="C62" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C63" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="E63" s="22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C63" s="21" t="s">
+    <row r="64" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C64" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="E64" s="22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C64" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D64" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="21">
         <v>7</v>
       </c>
@@ -2262,13 +2311,13 @@
         <v>24</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="21">
         <v>8</v>
       </c>
@@ -2276,36 +2325,36 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B67" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="A6:A41"/>
+    <mergeCell ref="B6:B41"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="E38:E41"/>
     <mergeCell ref="A42:A52"/>
     <mergeCell ref="B42:B52"/>
     <mergeCell ref="C47:C51"/>
-    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E47:E51"/>
     <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="A6:A41"/>
-    <mergeCell ref="B6:B41"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="D16:D21"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E42:E44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="256" scale="67" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="256" scale="38" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2316,7 +2365,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se han añadido las variables de entrada y salida para los momentos, elección poste, elección cimentación y péndola.
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Organización H" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Organización T'!$A$3:$I$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Organización T'!$A$3:$I$89</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="138">
   <si>
     <t>Días laborables</t>
   </si>
@@ -199,12 +199,6 @@
   </si>
   <si>
     <t>Comprobación del buen funcionamiento de la herramienta</t>
-  </si>
-  <si>
-    <t>Cálculo del momento realizado por el sistema de catenaria</t>
-  </si>
-  <si>
-    <t>Elección del poste adecuado que soporte el momento realizado por la catenaria</t>
   </si>
   <si>
     <t>Elección de la cimentación adecuada que soporte el momento realizado por la catenaria</t>
@@ -351,6 +345,102 @@
   </si>
   <si>
     <t>Funciones</t>
+  </si>
+  <si>
+    <t>Cálculo del momento al que está sometido cada poste</t>
+  </si>
+  <si>
+    <t>Elección del poste en base al momento calculado</t>
+  </si>
+  <si>
+    <t>vano anterior y posterior</t>
+  </si>
+  <si>
+    <t>velocidad viento</t>
+  </si>
+  <si>
+    <t>diametros conductores</t>
+  </si>
+  <si>
+    <t>pesos conductores</t>
+  </si>
+  <si>
+    <t>tensiones conductores</t>
+  </si>
+  <si>
+    <t>número conductores</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>distancias verticales y horizontales de los conductores y del equipamiento a la base del poste</t>
+  </si>
+  <si>
+    <t>descentramientos</t>
+  </si>
+  <si>
+    <t>Características de todos los tipos de postes existentes para la concepción de la catenaria en estudio</t>
+  </si>
+  <si>
+    <t>momento resultante en cada poste</t>
+  </si>
+  <si>
+    <t>momento resultante del poste seleccionado</t>
+  </si>
+  <si>
+    <t>tipo de vano (seccionamientos, agujas, zona neutra, sep.sistemas)</t>
+  </si>
+  <si>
+    <t>elevaciones si existen a lado y lado del vano</t>
+  </si>
+  <si>
+    <t>vano</t>
+  </si>
+  <si>
+    <t>peso aisladores de sección o de zona neutra</t>
+  </si>
+  <si>
+    <t>tensión conductores</t>
+  </si>
+  <si>
+    <t>peso conductores</t>
+  </si>
+  <si>
+    <t>flecha inicial</t>
+  </si>
+  <si>
+    <t>distancia entre primera y segunda péndola</t>
+  </si>
+  <si>
+    <t>distancia entre el apoyo y la primera péndola</t>
+  </si>
+  <si>
+    <t>distancia entre segunda y tercera péndola (opcional)</t>
+  </si>
+  <si>
+    <t>distancia máxima entre péndolas</t>
+  </si>
+  <si>
+    <t>longitud mínima de las péndolas</t>
+  </si>
+  <si>
+    <t>peso del conjunto de la péndola</t>
+  </si>
+  <si>
+    <t>función que obtiene el momento resultante según el equipamiento, condutores y condiciones del trazado para cada poste.</t>
+  </si>
+  <si>
+    <t>función que aporta el tipo de poste así como el momento máximo que es capaz de soportar</t>
+  </si>
+  <si>
+    <t>función que aporta el tipo de cimentación adecuada para el tipo de poste seleccionado</t>
+  </si>
+  <si>
+    <t>función que aporta las distancias a las que se situan en el vano las péndolas y la longitud que corresponde a cada una de ellas según la flecha de hilo(s) y sustentador</t>
+  </si>
+  <si>
+    <t>distancia en apoyo entre hilo(s) y susentador</t>
   </si>
 </sst>
 </file>
@@ -567,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -645,6 +735,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -955,13 +1057,13 @@
       <selection activeCell="C3" sqref="C3:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -969,7 +1071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
       <c r="C3" s="16" t="s">
         <v>16</v>
@@ -1008,7 +1110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1156,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>15</v>
       </c>
@@ -1084,7 +1186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
@@ -1126,7 +1228,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1139,7 +1241,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
@@ -1181,7 +1283,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>17</v>
       </c>
@@ -1223,7 +1325,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1236,7 +1338,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="13" t="s">
         <v>16</v>
@@ -1269,7 +1371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1309,7 +1411,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>15</v>
       </c>
@@ -1339,7 +1441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
@@ -1381,7 +1483,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1394,7 +1496,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
@@ -1489,27 +1591,27 @@
   <sheetPr codeName="Hoja2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I67"/>
+  <dimension ref="A2:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B73" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="21" customWidth="1"/>
     <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="24" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="21" customWidth="1"/>
     <col min="6" max="6" width="35" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
@@ -1517,10 +1619,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>48</v>
@@ -1529,16 +1631,16 @@
         <v>26</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>47</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>1</v>
       </c>
@@ -1546,7 +1648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>2</v>
       </c>
@@ -1554,339 +1656,339 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
         <v>3</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="23"/>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="21" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="27"/>
+      <c r="H8" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="21" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="27"/>
+      <c r="H9" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="26"/>
-      <c r="H8" s="21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="26"/>
-      <c r="H9" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="23"/>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="27" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10" s="21">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="23"/>
-      <c r="E11" s="26"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I11" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="26"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I12" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="26"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="27"/>
+      <c r="H14" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="27"/>
+      <c r="H15" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="26"/>
-      <c r="H14" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="26"/>
-      <c r="H15" s="21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>95</v>
-      </c>
       <c r="H16" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I16" s="21">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="23"/>
-      <c r="E17" s="26"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I17" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="23"/>
-      <c r="E18" s="26"/>
+      <c r="E18" s="27"/>
       <c r="F18" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I18" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="23"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H19" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="21" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="21" t="s">
+      <c r="H20" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>95</v>
-      </c>
       <c r="H22" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" s="21">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="23"/>
-      <c r="E23" s="26"/>
+      <c r="E23" s="27"/>
       <c r="F23" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I23" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="23"/>
-      <c r="E24" s="26"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I24" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="23"/>
-      <c r="E25" s="26"/>
+      <c r="E25" s="27"/>
       <c r="F25" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H25" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="21" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="21" t="s">
-        <v>93</v>
-      </c>
       <c r="H26" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="25"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="23"/>
-      <c r="E27" s="26"/>
+      <c r="E27" s="27"/>
       <c r="F27" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I27" s="21">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26"/>
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="22" t="s">
         <v>35</v>
       </c>
@@ -1895,226 +1997,226 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
-      <c r="B30" s="26"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="23"/>
-      <c r="E31" s="26" t="s">
-        <v>84</v>
+      <c r="E31" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I31" s="21">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="23"/>
-      <c r="E32" s="26"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I32" s="21">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="23"/>
-      <c r="E33" s="26"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I33" s="21">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="23"/>
-      <c r="E34" s="26"/>
+      <c r="E34" s="27"/>
       <c r="H34" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I34" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="23"/>
-      <c r="E35" s="26"/>
+      <c r="E35" s="27"/>
       <c r="H35" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I35" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="22" t="s">
-        <v>87</v>
-      </c>
       <c r="H37" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I37" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26" t="s">
+    <row r="38" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="23"/>
-      <c r="E38" s="26" t="s">
-        <v>88</v>
+      <c r="E38" s="27" t="s">
+        <v>86</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I38" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="23"/>
-      <c r="E39" s="26"/>
+      <c r="E39" s="27"/>
       <c r="F39" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I39" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="23"/>
-      <c r="E40" s="26"/>
+      <c r="E40" s="27"/>
       <c r="F40" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="25"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="23"/>
-      <c r="E41" s="26"/>
+      <c r="E41" s="27"/>
       <c r="H41" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="28">
         <v>4</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="27" t="s">
         <v>54</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I42" s="21">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="25"/>
-      <c r="E43" s="26"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="E43" s="27"/>
       <c r="F43" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="25"/>
-      <c r="E44" s="26"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+      <c r="E44" s="27"/>
       <c r="F44" s="22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="25"/>
-      <c r="B45" s="26"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="21" t="s">
         <v>38</v>
       </c>
@@ -2122,9 +2224,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
-      <c r="B46" s="26"/>
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="21" t="s">
         <v>39</v>
       </c>
@@ -2132,114 +2234,114 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="25"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="25" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E47" s="27" t="s">
         <v>57</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I47" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="25"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="25"/>
-      <c r="E48" s="26"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="28"/>
+      <c r="E48" s="27"/>
       <c r="F48" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I48" s="21">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="25"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="25"/>
-      <c r="E49" s="26"/>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="28"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="E49" s="27"/>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I49" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="25"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="25"/>
-      <c r="E50" s="26"/>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="28"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="E50" s="27"/>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I50" s="21">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="25"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="25"/>
-      <c r="E51" s="26"/>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="28"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
       <c r="H51" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I51" s="21">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="25"/>
-      <c r="B52" s="26"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="28"/>
+      <c r="B52" s="27"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E55" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
     </row>
-    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="21">
         <v>5</v>
       </c>
@@ -2247,7 +2349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C58" s="21" t="s">
         <v>45</v>
       </c>
@@ -2255,14 +2357,14 @@
         <v>58</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C59" s="21" t="s">
         <v>46</v>
       </c>
@@ -2270,7 +2372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="21">
         <v>6</v>
       </c>
@@ -2278,58 +2380,396 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="22"/>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E62" s="22" t="s">
+      <c r="E62" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F62" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H62" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63" s="25"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="25"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="25"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G64" s="25"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="25"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="25"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G65" s="25"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="25"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="25"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="G66" s="25"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="25"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="25"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="27"/>
+      <c r="F67" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G67" s="25"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="25"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="25"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G68" s="25"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="25"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="25"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G69" s="25"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="25"/>
+    </row>
+    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="25"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="27"/>
+      <c r="F70" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="G70" s="25"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="25"/>
+    </row>
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="H71" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="25"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="25"/>
+      <c r="H72" s="30"/>
+      <c r="I72" s="25"/>
+    </row>
+    <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C73" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" s="22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C63" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E63" s="22" t="s">
+      <c r="F73" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="H73" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="21">
+        <v>7</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" s="27" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C64" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="21">
-        <v>7</v>
-      </c>
-      <c r="B65" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="21">
+      <c r="F74" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="H74" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="25"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="G75" s="25"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="25"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="25"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G76" s="25"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="25"/>
+    </row>
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="25"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="G77" s="25"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="25"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="25"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="27"/>
+      <c r="F78" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G78" s="25"/>
+      <c r="H78" s="30"/>
+      <c r="I78" s="25"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="25"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="27"/>
+      <c r="F79" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="G79" s="25"/>
+      <c r="H79" s="30"/>
+      <c r="I79" s="25"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="25"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="27"/>
+      <c r="F80" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G80" s="25"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="25"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="25"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G81" s="25"/>
+      <c r="H81" s="30"/>
+      <c r="I81" s="25"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="25"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="27"/>
+      <c r="F82" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G82" s="25"/>
+      <c r="H82" s="30"/>
+      <c r="I82" s="25"/>
+    </row>
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="25"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="G83" s="25"/>
+      <c r="H83" s="30"/>
+      <c r="I83" s="25"/>
+    </row>
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="25"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G84" s="25"/>
+      <c r="H84" s="30"/>
+      <c r="I84" s="25"/>
+    </row>
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="25"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="27"/>
+      <c r="F85" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="G85" s="25"/>
+      <c r="H85" s="30"/>
+      <c r="I85" s="25"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="25"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="27"/>
+      <c r="F86" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="G86" s="25"/>
+      <c r="H86" s="30"/>
+      <c r="I86" s="25"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="25"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G87" s="25"/>
+      <c r="H87" s="30"/>
+      <c r="I87" s="25"/>
+    </row>
+    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="25"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="G88" s="25"/>
+      <c r="H88" s="30"/>
+      <c r="I88" s="25"/>
+    </row>
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="21">
         <v>8</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="B89" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="22"/>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="31">
+    <mergeCell ref="H62:H70"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="H74:H88"/>
+    <mergeCell ref="C62:C70"/>
+    <mergeCell ref="E62:E70"/>
+    <mergeCell ref="E74:E88"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C74:C88"/>
+    <mergeCell ref="A42:A52"/>
+    <mergeCell ref="B42:B52"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="E42:E44"/>
     <mergeCell ref="C22:C27"/>
     <mergeCell ref="E22:E27"/>
     <mergeCell ref="A6:A41"/>
@@ -2346,12 +2786,6 @@
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="C38:C41"/>
     <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A42:A52"/>
-    <mergeCell ref="B42:B52"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="E42:E44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="256" scale="38" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2365,7 +2799,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>